<commit_message>
Updated publish profile. Updated excel file and instructions in the ImportExcel tool.
</commit_message>
<xml_diff>
--- a/Basiscore.Minions/sitecore/admin/minions/assets/files/ImportExcelDataSample.xlsx
+++ b/Basiscore.Minions/sitecore/admin/minions/assets/files/ImportExcelDataSample.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25726"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06C39599-FA7E-4A45-A0C7-94D4D7499274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="5" r:id="rId1"/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>ITEM_NAME</t>
   </si>
@@ -37,39 +38,15 @@
     <t>CA</t>
   </si>
   <si>
-    <t>{999F3376-8F16-42EE-8B87-85218F37A10E}</t>
-  </si>
-  <si>
-    <t>{52E425E7-A2F2-4669-A683-4FCB9376ED8E}</t>
-  </si>
-  <si>
     <t>Canada</t>
   </si>
   <si>
-    <t>Code</t>
-  </si>
-  <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>Currency</t>
-  </si>
-  <si>
     <t>Quebec</t>
   </si>
   <si>
-    <t>USD</t>
-  </si>
-  <si>
-    <t>CAD</t>
-  </si>
-  <si>
     <t>12 USD/Hr</t>
   </si>
   <si>
-    <t>QC</t>
-  </si>
-  <si>
     <t>12.5 CAD/Hr</t>
   </si>
   <si>
@@ -82,13 +59,37 @@
     <t>/sitecore/content/Countries/Canada</t>
   </si>
   <si>
-    <t>Minimum Wage</t>
+    <t>Countries</t>
+  </si>
+  <si>
+    <t>{A87A00B1-E6DB-45AB-8B54-636FEC3B5523}</t>
+  </si>
+  <si>
+    <t>/sitecore/content</t>
+  </si>
+  <si>
+    <t>{A08790DA-FAE8-4DDA-A4F8-CFE38EACE722}</t>
+  </si>
+  <si>
+    <t>Country Code</t>
+  </si>
+  <si>
+    <t>{6D1CD897-1936-4A3A-A511-289A94C2A7B1}</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>Phrase</t>
+  </si>
+  <si>
+    <t>Minium Wage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -168,6 +169,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -215,7 +219,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -248,9 +252,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -283,6 +304,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -458,11 +496,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,14 +508,13 @@
     <col min="1" max="1" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="56.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -488,97 +525,88 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="D3" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>